<commit_message>
update Marking Scheme checklist
</commit_message>
<xml_diff>
--- a/Documentation/Marking Scheme.xlsx
+++ b/Documentation/Marking Scheme.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aston\Documents\GitHub\GP3\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A663F059-AD8B-4ED3-B3A1-B938430A9593}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC944B3-8560-41FE-9A6B-FFA69D933DB8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="760" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28005" yWindow="0" windowWidth="26130" windowHeight="15315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
   <si>
     <t xml:space="preserve">Team Code : </t>
   </si>
@@ -358,6 +358,9 @@
   </si>
   <si>
     <t>cancel a booking</t>
+  </si>
+  <si>
+    <t>members can</t>
   </si>
 </sst>
 </file>
@@ -478,7 +481,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -709,9 +712,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -798,30 +798,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1105,21 +1108,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F285"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.54296875" customWidth="1"/>
-    <col min="2" max="2" width="74.453125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" customWidth="1"/>
+    <col min="2" max="2" width="74.42578125" style="3" customWidth="1"/>
     <col min="3" max="3" width="7" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.81640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="71.1796875" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="71.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="42" t="s">
         <v>84</v>
       </c>
@@ -1127,64 +1130,64 @@
       <c r="C1" s="42"/>
       <c r="D1" s="42"/>
     </row>
-    <row r="2" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="43" t="s">
+    <row r="3" spans="1:6" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-    </row>
-    <row r="4" spans="1:6" s="8" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="40" t="s">
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+    </row>
+    <row r="4" spans="1:6" s="7" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-    </row>
-    <row r="5" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+    </row>
+    <row r="5" spans="1:6" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="38" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1.2</v>
       </c>
-      <c r="B6" s="45" t="s">
+      <c r="B6" s="39" t="s">
         <v>42</v>
       </c>
       <c r="D6" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6" t="s">
+    <row r="7" spans="1:6" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <f>SUM(C5:C6)</f>
         <v>0</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="6">
         <f>SUM(D5:D6)</f>
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="41" t="s">
         <v>47</v>
       </c>
@@ -1192,23 +1195,23 @@
       <c r="C8" s="41"/>
       <c r="D8" s="41"/>
     </row>
-    <row r="9" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="13">
+    <row r="9" spans="1:6" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="12">
         <v>2.1</v>
       </c>
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="39" t="s">
         <v>45</v>
       </c>
       <c r="D9" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="13">
+    <row r="10" spans="1:6" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="12">
         <f>A9+0.1</f>
         <v>2.2000000000000002</v>
       </c>
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="39" t="s">
         <v>58</v>
       </c>
       <c r="D10" s="1">
@@ -1216,114 +1219,117 @@
       </c>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="13">
+    <row r="11" spans="1:6" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
         <f t="shared" ref="A11:A12" si="0">A10+0.1</f>
         <v>2.3000000000000003</v>
       </c>
-      <c r="B11" s="45" t="s">
+      <c r="B11" s="39" t="s">
         <v>62</v>
       </c>
       <c r="D11" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="13">
+      <c r="F11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
         <f t="shared" si="0"/>
         <v>2.4000000000000004</v>
       </c>
-      <c r="B12" s="45" t="s">
+      <c r="B12" s="39" t="s">
         <v>46</v>
       </c>
       <c r="D12" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="13">
+    <row r="13" spans="1:6" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
         <f>A12+0.1</f>
         <v>2.5000000000000004</v>
       </c>
-      <c r="B13" s="45" t="s">
+      <c r="B13" s="39" t="s">
         <v>71</v>
       </c>
       <c r="D13" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="13">
+    <row r="14" spans="1:6" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
         <f>A13+0.1</f>
         <v>2.6000000000000005</v>
       </c>
-      <c r="B14" s="45" t="s">
+      <c r="B14" s="39" t="s">
         <v>59</v>
       </c>
       <c r="D14" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="13">
+    <row r="15" spans="1:6" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="12">
         <f>A14+0.1</f>
         <v>2.7000000000000006</v>
       </c>
-      <c r="B15" s="45" t="s">
+      <c r="B15" s="39" t="s">
         <v>60</v>
       </c>
       <c r="D15" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="5"/>
-      <c r="B16" s="6" t="s">
+    <row r="16" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="6">
         <f ca="1">SUM(C9:C24)</f>
         <v>0</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="6">
         <f>SUM(D9:D15)</f>
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="8" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="40" t="s">
+    <row r="17" spans="1:4" s="7" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="40"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-    </row>
-    <row r="18" spans="1:4" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="13">
+      <c r="B17" s="43"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
+    </row>
+    <row r="18" spans="1:4" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="12">
         <v>3.1</v>
       </c>
-      <c r="B18" s="45" t="s">
+      <c r="B18" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="31"/>
+      <c r="C18" s="30"/>
       <c r="D18" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="13">
+    <row r="19" spans="1:4" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="12">
         <f>A18+0.1</f>
         <v>3.2</v>
       </c>
-      <c r="B19" s="45" t="s">
+      <c r="B19" s="39" t="s">
         <v>72</v>
       </c>
       <c r="D19" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="13">
+    <row r="20" spans="1:4" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="12">
         <f t="shared" ref="A20:A24" si="1">A19+0.1</f>
         <v>3.3000000000000003</v>
       </c>
@@ -1334,20 +1340,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="13">
+    <row r="21" spans="1:4" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="12">
         <f t="shared" si="1"/>
         <v>3.4000000000000004</v>
       </c>
-      <c r="B21" s="45" t="s">
+      <c r="B21" s="39" t="s">
         <v>63</v>
       </c>
       <c r="D21" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="13">
+    <row r="22" spans="1:4" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="12">
         <f t="shared" si="1"/>
         <v>3.5000000000000004</v>
       </c>
@@ -1358,109 +1364,109 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="13">
+    <row r="23" spans="1:4" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="12">
         <f t="shared" si="1"/>
         <v>3.6000000000000005</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="39" t="s">
         <v>65</v>
       </c>
       <c r="D23" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="13">
+    <row r="24" spans="1:4" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="12">
         <f t="shared" si="1"/>
         <v>3.7000000000000006</v>
       </c>
-      <c r="B24" s="47" t="s">
+      <c r="B24" s="40" t="s">
         <v>73</v>
       </c>
       <c r="D24" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6" t="s">
+    <row r="25" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C25" s="6">
         <f>SUM(C19:C24)</f>
         <v>0</v>
       </c>
-      <c r="D25" s="7">
+      <c r="D25" s="6">
         <f>SUM(D18:D24)</f>
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="39" t="s">
+    <row r="26" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="B26" s="39"/>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
-    </row>
-    <row r="27" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="13">
+      <c r="B26" s="45"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+    </row>
+    <row r="27" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="12">
         <v>4.0999999999999996</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C27" s="26"/>
-      <c r="D27" s="27">
+      <c r="C27" s="25"/>
+      <c r="D27" s="26">
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="13">
+    <row r="28" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="12">
         <f>A27+0.1</f>
         <v>4.1999999999999993</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="C28" s="26"/>
-      <c r="D28" s="27">
+      <c r="C28" s="25"/>
+      <c r="D28" s="26">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="13">
+    <row r="29" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="12">
         <f>A28+0.1</f>
         <v>4.2999999999999989</v>
       </c>
-      <c r="B29" s="44" t="s">
+      <c r="B29" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="C29" s="26"/>
-      <c r="D29" s="27">
+      <c r="C29" s="25"/>
+      <c r="D29" s="26">
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="13">
+    <row r="30" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="12">
         <f t="shared" ref="A30:A33" si="2">A29+0.1</f>
         <v>4.3999999999999986</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="C30" s="26"/>
+      <c r="C30" s="25"/>
       <c r="D30" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="13">
+    <row r="31" spans="1:4" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="12">
         <f t="shared" si="2"/>
         <v>4.4999999999999982</v>
       </c>
-      <c r="B31" s="44" t="s">
+      <c r="B31" s="38" t="s">
         <v>74</v>
       </c>
       <c r="C31"/>
@@ -1468,12 +1474,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="13">
+    <row r="32" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="12">
         <f t="shared" si="2"/>
         <v>4.5999999999999979</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="47" t="s">
         <v>76</v>
       </c>
       <c r="C32"/>
@@ -1481,12 +1487,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="13">
+    <row r="33" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="12">
         <f t="shared" si="2"/>
         <v>4.6999999999999975</v>
       </c>
-      <c r="B33" s="44" t="s">
+      <c r="B33" s="38" t="s">
         <v>40</v>
       </c>
       <c r="C33"/>
@@ -1497,32 +1503,32 @@
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="3" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="37"/>
-      <c r="B34" s="33" t="s">
+    <row r="34" spans="1:6" s="3" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="36"/>
+      <c r="B34" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="C34" s="34">
+      <c r="C34" s="33">
         <f>SUM(C31:C33)</f>
         <v>0</v>
       </c>
-      <c r="D34" s="34">
+      <c r="D34" s="33">
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:6" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="39" t="s">
+    <row r="35" spans="1:6" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="45" t="s">
         <v>52</v>
       </c>
-      <c r="B35" s="39"/>
-      <c r="C35" s="30"/>
-      <c r="D35" s="30"/>
-    </row>
-    <row r="36" spans="1:6" s="3" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B35" s="45"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="29"/>
+    </row>
+    <row r="36" spans="1:6" s="3" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>53</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="39" t="s">
         <v>77</v>
       </c>
       <c r="C36" s="1"/>
@@ -1530,11 +1536,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="36" t="s">
+    <row r="37" spans="1:6" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="46" t="s">
         <v>78</v>
       </c>
       <c r="C37" s="1"/>
@@ -1542,60 +1548,60 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:6" s="3" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="15"/>
-      <c r="B38" s="33" t="s">
+    <row r="38" spans="1:6" s="3" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="14"/>
+      <c r="B38" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="C38" s="35"/>
-      <c r="D38" s="35">
+      <c r="C38" s="34"/>
+      <c r="D38" s="34">
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:6" s="3" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="5"/>
-      <c r="B39" s="6" t="s">
+    <row r="39" spans="1:6" s="3" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="4"/>
+      <c r="B39" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C39" s="7">
+      <c r="C39" s="6">
         <f ca="1">C7+C25+C16+C34</f>
         <v>0</v>
       </c>
-      <c r="D39" s="7">
+      <c r="D39" s="6">
         <f>D7+D25+D16+D34+D38</f>
         <v>75</v>
       </c>
     </row>
-    <row r="40" spans="1:6" s="3" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="29" t="s">
+    <row r="40" spans="1:6" s="3" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="B40" s="29"/>
-      <c r="C40" s="29"/>
-      <c r="D40" s="29"/>
-    </row>
-    <row r="41" spans="1:6" s="3" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="40" t="s">
+      <c r="B40" s="28"/>
+      <c r="C40" s="28"/>
+      <c r="D40" s="28"/>
+    </row>
+    <row r="41" spans="1:6" s="3" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="B41" s="40"/>
-      <c r="C41" s="28"/>
-      <c r="D41" s="28"/>
-    </row>
-    <row r="42" spans="1:6" s="3" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="38">
+      <c r="B41" s="43"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="27"/>
+    </row>
+    <row r="42" spans="1:6" s="3" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="37">
         <v>6.1</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>68</v>
       </c>
       <c r="C42"/>
-      <c r="D42" s="10">
+      <c r="D42" s="9">
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="38">
+    <row r="43" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="37">
         <f>A42+0.1</f>
         <v>6.1999999999999993</v>
       </c>
@@ -1603,12 +1609,12 @@
         <v>69</v>
       </c>
       <c r="C43"/>
-      <c r="D43" s="10">
+      <c r="D43" s="9">
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:6" s="3" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="38">
+    <row r="44" spans="1:6" s="3" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="37">
         <f t="shared" ref="A44:A46" si="3">A43+0.1</f>
         <v>6.2999999999999989</v>
       </c>
@@ -1616,12 +1622,12 @@
         <v>51</v>
       </c>
       <c r="C44"/>
-      <c r="D44" s="10">
+      <c r="D44" s="9">
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:6" s="3" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="38">
+    <row r="45" spans="1:6" s="3" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="37">
         <f t="shared" si="3"/>
         <v>6.3999999999999986</v>
       </c>
@@ -1629,12 +1635,12 @@
         <v>6</v>
       </c>
       <c r="C45"/>
-      <c r="D45" s="10">
+      <c r="D45" s="9">
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:6" s="3" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="38">
+    <row r="46" spans="1:6" s="3" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="37">
         <f t="shared" si="3"/>
         <v>6.4999999999999982</v>
       </c>
@@ -1642,66 +1648,66 @@
         <v>7</v>
       </c>
       <c r="C46"/>
-      <c r="D46" s="10">
+      <c r="D46" s="9">
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:6" s="3" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="11"/>
-      <c r="B47" s="12" t="s">
+    <row r="47" spans="1:6" s="3" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="10"/>
+      <c r="B47" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C47" s="7">
+      <c r="C47" s="6">
         <f>SUM(C42:C46)</f>
         <v>0</v>
       </c>
-      <c r="D47" s="7">
+      <c r="D47" s="6">
         <f>SUM(D42:D46)</f>
         <v>24</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="32" t="s">
+    <row r="48" spans="1:6" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="B48" s="32"/>
-      <c r="C48" s="32"/>
-      <c r="D48" s="32"/>
-    </row>
-    <row r="49" spans="1:4" s="3" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="40" t="s">
+      <c r="B48" s="31"/>
+      <c r="C48" s="31"/>
+      <c r="D48" s="31"/>
+    </row>
+    <row r="49" spans="1:4" s="3" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="B49" s="40"/>
-      <c r="C49" s="28"/>
-      <c r="D49" s="28"/>
-    </row>
-    <row r="50" spans="1:4" s="3" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="38">
+      <c r="B49" s="43"/>
+      <c r="C49" s="27"/>
+      <c r="D49" s="27"/>
+    </row>
+    <row r="50" spans="1:4" s="3" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="37">
         <v>6.6</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C50" s="2"/>
-      <c r="D50" s="9">
+      <c r="D50" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="38">
+    <row r="51" spans="1:4" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="37">
         <v>6.2</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C51" s="2"/>
-      <c r="D51" s="9">
+      <c r="D51" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A52" s="38">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="37">
         <v>6.3</v>
       </c>
       <c r="B52" s="2" t="s">
@@ -1711,522 +1717,522 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:4" s="2" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="11"/>
-      <c r="B53" s="12" t="s">
+    <row r="53" spans="1:4" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="10"/>
+      <c r="B53" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C53" s="7">
+      <c r="C53" s="6">
         <f>SUM(C60:C62)</f>
         <v>0</v>
       </c>
-      <c r="D53" s="7">
+      <c r="D53" s="6">
         <f>SUM(D50:D52)</f>
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:4" s="2" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="32" t="s">
+    <row r="54" spans="1:4" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="B54" s="32"/>
-      <c r="C54" s="32"/>
-      <c r="D54" s="32"/>
-    </row>
-    <row r="55" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="40" t="s">
+      <c r="B54" s="31"/>
+      <c r="C54" s="31"/>
+      <c r="D54" s="31"/>
+    </row>
+    <row r="55" spans="1:4" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="B55" s="40"/>
-      <c r="C55" s="28"/>
-      <c r="D55" s="28"/>
-    </row>
-    <row r="56" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="38">
+      <c r="B55" s="43"/>
+      <c r="C55" s="27"/>
+      <c r="D55" s="27"/>
+    </row>
+    <row r="56" spans="1:4" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="37">
         <v>7.1</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>70</v>
       </c>
       <c r="C56" s="2"/>
-      <c r="D56" s="9">
+      <c r="D56" s="8">
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="38">
+    <row r="57" spans="1:4" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="37">
         <v>7.2</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C57" s="2"/>
-      <c r="D57" s="9">
+      <c r="D57" s="8">
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="38">
+    <row r="58" spans="1:4" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="37">
         <v>7.3</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>80</v>
       </c>
       <c r="C58" s="2"/>
-      <c r="D58" s="9">
+      <c r="D58" s="8">
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="38">
+    <row r="59" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="37">
         <v>7.4</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>57</v>
       </c>
       <c r="C59" s="2"/>
-      <c r="D59" s="9"/>
-    </row>
-    <row r="60" spans="1:4" s="3" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D59" s="8"/>
+    </row>
+    <row r="60" spans="1:4" s="3" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C60" s="9"/>
-      <c r="D60" s="9">
+      <c r="C60" s="8"/>
+      <c r="D60" s="8">
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:4" s="3" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" s="3" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C61" s="9"/>
-      <c r="D61" s="9">
+      <c r="C61" s="8"/>
+      <c r="D61" s="8">
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:4" s="2" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" s="2" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
       <c r="B62" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C62" s="9"/>
-      <c r="D62" s="9">
+      <c r="C62" s="8"/>
+      <c r="D62" s="8">
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="11"/>
-      <c r="B63" s="12" t="s">
+    <row r="63" spans="1:4" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="10"/>
+      <c r="B63" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C63" s="7">
+      <c r="C63" s="6">
         <f>SUM(C56:C58)</f>
         <v>0</v>
       </c>
-      <c r="D63" s="7">
+      <c r="D63" s="6">
         <f>SUM(D56:D62)</f>
         <v>45</v>
       </c>
     </row>
-    <row r="64" spans="1:4" s="2" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="11"/>
-      <c r="B64" s="12" t="s">
+    <row r="64" spans="1:4" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="10"/>
+      <c r="B64" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C64" s="7">
+      <c r="C64" s="6">
         <f ca="1">C39+C47+C53+C63</f>
         <v>0</v>
       </c>
-      <c r="D64" s="7">
+      <c r="D64" s="6">
         <f>D39+D47+D53+D63</f>
         <v>150</v>
       </c>
     </row>
-    <row r="65" spans="1:5" s="2" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="11"/>
-      <c r="B65" s="12" t="s">
+    <row r="65" spans="1:5" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="10"/>
+      <c r="B65" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C65" s="7">
+      <c r="C65" s="6">
         <f ca="1">C64/150*100</f>
         <v>0</v>
       </c>
-      <c r="D65" s="7">
+      <c r="D65" s="6">
         <f>D64/150*100</f>
         <v>100</v>
       </c>
       <c r="E65"/>
     </row>
-    <row r="66" spans="1:5" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="11"/>
-      <c r="B66" s="12" t="s">
+    <row r="66" spans="1:5" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="10"/>
+      <c r="B66" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C66" s="7">
+      <c r="C66" s="6">
         <f ca="1">C65/5</f>
         <v>0</v>
       </c>
-      <c r="D66" s="7">
+      <c r="D66" s="6">
         <f>D65/5</f>
         <v>20</v>
       </c>
       <c r="E66"/>
     </row>
-    <row r="67" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67"/>
       <c r="C67"/>
       <c r="D67"/>
     </row>
-    <row r="68" spans="1:5" s="2" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B68" s="14" t="s">
+    <row r="68" spans="1:5" s="2" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B68" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C68" s="16"/>
-      <c r="D68" s="9"/>
+      <c r="C68" s="15"/>
+      <c r="D68" s="8"/>
       <c r="E68"/>
     </row>
-    <row r="69" spans="1:5" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B69" s="18" t="s">
+    <row r="69" spans="1:5" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B69" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C69" s="19" t="s">
+      <c r="C69" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D69" s="20" t="str">
+      <c r="D69" s="19" t="str">
         <f ca="1">IF($C$65&gt;=79.5,"√","")</f>
         <v/>
       </c>
       <c r="E69"/>
     </row>
-    <row r="70" spans="1:5" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B70" s="21" t="s">
+    <row r="70" spans="1:5" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C70" s="17" t="s">
+      <c r="C70" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D70" s="22" t="str">
+      <c r="D70" s="21" t="str">
         <f ca="1">IF($C$65&lt;69.5," ",IF($C$65&lt;79.5,"√",""))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E70"/>
     </row>
-    <row r="71" spans="1:5" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B71" s="21" t="s">
+    <row r="71" spans="1:5" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C71" s="17" t="s">
+      <c r="C71" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D71" s="22" t="str">
+      <c r="D71" s="21" t="str">
         <f ca="1">IF($C$65&lt;59.5," ",IF($C$65&lt;69.5,"√",""))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E71"/>
     </row>
-    <row r="72" spans="1:5" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B72" s="21" t="s">
+    <row r="72" spans="1:5" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B72" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C72" s="17" t="s">
+      <c r="C72" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D72" s="22" t="str">
+      <c r="D72" s="21" t="str">
         <f ca="1">IF($C$65&lt;49.5," ",IF($C$65&lt;59.5,"√",""))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E72"/>
     </row>
-    <row r="73" spans="1:5" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="21" t="s">
+    <row r="73" spans="1:5" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B73" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C73" s="17" t="s">
+      <c r="C73" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="D73" s="22" t="str">
+      <c r="D73" s="21" t="str">
         <f ca="1">IF($C$65&lt;39.5," ",IF($C$65&lt;49.5,"√",""))</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="74" spans="1:5" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="21" t="s">
+    <row r="74" spans="1:5" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B74" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="C74" s="17" t="s">
+      <c r="C74" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D74" s="22" t="str">
+      <c r="D74" s="21" t="str">
         <f ca="1">IF($C$65&lt;29.5," ",IF($C$65&lt;39.5,"√",""))</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="75" spans="1:5" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="21" t="s">
+    <row r="75" spans="1:5" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B75" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="C75" s="17" t="s">
+      <c r="C75" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="D75" s="22" t="str">
+      <c r="D75" s="21" t="str">
         <f ca="1">IF($C$65&lt;19.5," ",IF($C$65&lt;29.5,"√",""))</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="76" spans="1:5" s="2" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="23" t="s">
+    <row r="76" spans="1:5" s="2" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B76" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="C76" s="24" t="s">
+      <c r="C76" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="D76" s="25" t="str">
+      <c r="D76" s="24" t="str">
         <f ca="1">IF($C$65&lt;0," ",IF($C$65&lt;19.5,"√",""))</f>
         <v>√</v>
       </c>
     </row>
-    <row r="77" spans="1:5" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="78" spans="1:5" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="79" spans="1:5" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="80" spans="1:5" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="81" spans="1:4" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="82" spans="1:4" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="83" spans="1:4" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="84" spans="1:4" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="85" spans="1:4" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="86" spans="1:4" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="87" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="1:5" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="1:5" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="1:5" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" spans="1:4" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" spans="1:4" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" spans="1:4" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" spans="1:4" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" spans="1:4" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" spans="1:4" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
       <c r="D87" s="2"/>
     </row>
-    <row r="88" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
       <c r="D88" s="2"/>
     </row>
-    <row r="89" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
       <c r="D89" s="2"/>
     </row>
-    <row r="90" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
       <c r="D90" s="2"/>
     </row>
-    <row r="91" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="92" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="93" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="94" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="95" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="96" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="97" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="98" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="99" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="100" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="101" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="102" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="103" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="104" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="105" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="106" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="107" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="108" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="109" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="110" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="111" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="112" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="113" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="114" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="115" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="116" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="117" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="118" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="119" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="120" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="121" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="122" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="123" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="124" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="125" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="126" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="127" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="128" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="129" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="130" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="131" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="132" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="133" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="134" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="135" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="136" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="137" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="138" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="139" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="140" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="141" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="142" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="143" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="144" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="145" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="146" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="147" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="148" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="149" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="150" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="151" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="152" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="153" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="154" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="155" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="156" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="157" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="158" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="159" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="160" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="161" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="162" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="163" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="164" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="165" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="166" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="167" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="168" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="169" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="170" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="171" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="172" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="173" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="174" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="175" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="176" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="177" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="178" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="179" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="180" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="181" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="182" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="183" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="184" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="185" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="186" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="187" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="188" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="189" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="190" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="191" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="192" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="193" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="194" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="195" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="196" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="197" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="198" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="199" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="200" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="201" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="202" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="203" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="204" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="205" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="206" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="207" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="208" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="209" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="210" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="211" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="212" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="213" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="214" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="215" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="216" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="217" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="218" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="219" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="220" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="221" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="222" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="223" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="224" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="225" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="226" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="227" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="228" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="229" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="230" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="231" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="232" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="233" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="234" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="235" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="236" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="237" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="238" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="239" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="240" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="241" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="242" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="243" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="244" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="245" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="246" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="247" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="248" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="249" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="250" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="251" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="252" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="253" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="254" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="255" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="256" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="257" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="258" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="259" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="260" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="261" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="262" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="263" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="264" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="265" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="266" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="267" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="268" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="269" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="270" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="271" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="272" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="273" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="274" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="275" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="276" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="277" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="278" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="279" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="280" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="281" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="282" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="283" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="284" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="285" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="91" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="101" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="102" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="103" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="104" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="107" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="108" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="109" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="110" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="113" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="114" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="115" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="116" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="119" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="126" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="127" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="128" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="129" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="130" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="131" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="132" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="133" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="134" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="135" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="136" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="137" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="138" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="139" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="140" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="141" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="142" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="143" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="144" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="145" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="146" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="147" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="148" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="149" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="150" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="151" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="152" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="153" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="154" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="155" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="157" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="158" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="160" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="161" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="162" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="163" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="164" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="165" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="166" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="167" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="168" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="169" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="170" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="171" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="172" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="173" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="174" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="175" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="176" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="177" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="178" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="179" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="180" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="181" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="182" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="183" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="184" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="185" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="186" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="187" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="188" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="189" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="190" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="191" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="192" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="193" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="194" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="195" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="196" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="197" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="198" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="199" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="200" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="201" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="202" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="203" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="204" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="205" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="206" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="207" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="208" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="209" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="210" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="211" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="212" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="213" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="214" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="215" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="216" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="217" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="218" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="219" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="220" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="221" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="222" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="223" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="224" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="225" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="226" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="227" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="228" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="229" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="230" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="231" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="232" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="233" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="234" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="235" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="236" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="237" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="238" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="239" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="240" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="241" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="242" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="243" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="244" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="245" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="246" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="247" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="248" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="249" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="250" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="251" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="252" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="253" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="254" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="255" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="256" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="257" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="258" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="259" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="260" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="261" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="262" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="263" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="264" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="265" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="266" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="267" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="268" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="269" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="270" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="271" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="272" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="273" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="274" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="275" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="276" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="277" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="278" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="279" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="280" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="281" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="282" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="283" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="284" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="285" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A35:B35"/>
     <mergeCell ref="A8:D8"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A35:B35"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.55118110236220474" bottom="0.55118110236220474" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>